<commit_message>
hierarchical name for org units Распределение 2021 07 июль.xlsx
</commit_message>
<xml_diff>
--- a/databases/xlsx/import_all/import 21.06.xlsx
+++ b/databases/xlsx/import_all/import 21.06.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="528">
   <si>
     <t xml:space="preserve">Организация</t>
   </si>
@@ -3339,12 +3339,12 @@
   <dimension ref="A1:I213"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="1" sqref="1:1 2:2"/>
+      <selection pane="bottomLeft" activeCell="G87" activeCellId="0" sqref="G87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="24.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="24.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="92.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.41"/>
@@ -5773,7 +5773,9 @@
       <c r="H99" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="I99" s="7"/>
+      <c r="I99" s="7" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="60"/>
@@ -8521,10 +8523,10 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="2" sqref="1:1 2:2 E6"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.85"/>

</xml_diff>